<commit_message>
attaché: valider et invalider session
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -13,13 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>assane cousin</t>
+    <t>ouseynou cousin</t>
   </si>
   <si>
-    <t>assane@gmail.com</t>
+    <t>ousseynou@gmail.com</t>
   </si>
   <si>
-    <t>assane</t>
+    <t>ousseynou</t>
   </si>
 </sst>
 </file>

</xml_diff>